<commit_message>
feat: able to loda data easily
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD0587F-568A-4979-B59D-E64908F8A99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE43C258-5A3D-413B-BFCD-FAFD3AEB64AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -74,7 +74,16 @@
 click on "Prescribe"</t>
   </si>
   <si>
-    <t>test</t>
+    <t>herbie_basic_test</t>
+  </si>
+  <si>
+    <t>enter firstname last name and click on submit verify whther its correct or not</t>
+  </si>
+  <si>
+    <t>https://mieweb.github.io/herbie/playgrounds/login.html</t>
+  </si>
+  <si>
+    <t>verify state is visible in "result"</t>
   </si>
 </sst>
 </file>
@@ -119,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -136,6 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,10 +489,10 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.25" customWidth="1"/>
     <col min="3" max="3" width="29.625" customWidth="1"/>
@@ -490,7 +500,7 @@
     <col min="5" max="5" width="39.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,21 +556,22 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{04ED3031-8870-4330-81D1-8617DD329C46}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{FE524888-D6D2-4840-9416-D3F21926355F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:E1 A3:B3 A2:B2 D2" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
feat: test doc update
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE43C258-5A3D-413B-BFCD-FAFD3AEB64AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169B103F-0EF0-49C3-8313-CF6F271736B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -488,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat: styling of renderd tests
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169B103F-0EF0-49C3-8313-CF6F271736B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D7DEB7-01D4-4055-A3B2-968B99953C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
     <t>https://mieweb.github.io/herbie/playgrounds/login.html</t>
   </si>
   <si>
-    <t>verify state is visible in "result"</t>
+    <t>verify url equals "https://mieweb.github.io/herbie/playgrounds/login.html"</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
iproved ui for tasks
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8297DB13-8FC7-448E-8EDE-5F7B1E2D9A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C8DBA9-57D7-4424-A840-A3F53C818B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +112,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -499,7 +505,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -544,49 +550,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="330.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="330.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{04ED3031-8870-4330-81D1-8617DD329C46}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{FE524888-D6D2-4840-9416-D3F21926355F}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{04ED3031-8870-4330-81D1-8617DD329C46}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{FE524888-D6D2-4840-9416-D3F21926355F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A3:B3 A2 D2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1 B4 A2 D2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: for basic test url
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBDB2A4-8A4A-4334-967A-47E1AB6AE6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0976CE8A-9545-475B-AE30-51232BA802AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -68,29 +68,13 @@
     <t>verify url equals "https://workforcenow.adp.com/theme/index.html#/Myself/empOrganizationalChart"</t>
   </si>
   <si>
-    <t>Objective: Test search and navigation skills.
-Task: Use the search bar to find a specific document (e.g., “2025 Academy Agenda”).</t>
-  </si>
-  <si>
-    <t>https://workspace.google.com/products/drive/</t>
-  </si>
-  <si>
-    <t>verify text equals "2025 Academy Agenda" in "Academy_agenda_file"</t>
-  </si>
-  <si>
     <t>Webchart Prescribe a Medicine</t>
   </si>
   <si>
     <t>ADP Task</t>
   </si>
   <si>
-    <t>Google Drive Task</t>
-  </si>
-  <si>
     <t>Webchart Select Patient Task</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/academy.html</t>
   </si>
   <si>
     <t xml:space="preserve">verify url equals "http://localhost:3000/academy.html"
@@ -102,6 +86,9 @@
   <si>
     <t>Objective: Demonstrate basic form interaction and submission skills.
 Task: Enter your name in the form and submit it in academy page.</t>
+  </si>
+  <si>
+    <t>http://18.219.226.248/academy.html</t>
   </si>
 </sst>
 </file>
@@ -513,7 +500,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -546,16 +533,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
@@ -563,7 +550,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -580,7 +567,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -597,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -609,22 +596,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
changed to master daily
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D9F804-A1FA-433B-AD65-A5ACBE04A30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8D8254-BD8C-40D7-BB83-5A6D28AEF79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -35,25 +35,12 @@
   </si>
   <si>
     <t>herbie_script</t>
-  </si>
-  <si>
-    <t>https://hrithik.webchartnow.com/webchart.cgi?f=chart</t>
-  </si>
-  <si>
-    <t>https://hrithik.webchartnow.com/webchart.cgi?f=chart&amp;s=pat&amp;pat_id=18</t>
   </si>
   <si>
     <t>Select Hart, William S from the list
 go to the charter page</t>
   </si>
   <si>
-    <t>Write Amoxicillin 500mg capsule 2 caps daily for 7 days. For Prescriber: Hrithik Mani. Total quantity: 14 and no refills. Allow substitutions Send the script to "MIE Test Pharmacy", for patient Manu Deepika</t>
-  </si>
-  <si>
-    <t>verify text equals "MANU, DEEPIKA" in "patient_name"
-verify text equals "amoxicillin 500 mg tablet" in "medicine"</t>
-  </si>
-  <si>
     <t>https://workforcenow.adp.com/theme/index.html#/home</t>
   </si>
   <si>
@@ -89,6 +76,16 @@
   <si>
     <t xml:space="preserve">
 verify text equals "HART, WILLIAM S." in "patient_name"</t>
+  </si>
+  <si>
+    <t>https://masterdaily.dev.webchart.app/webchart.cgi</t>
+  </si>
+  <si>
+    <t>Write Amoxicillin 500mg capsule 2 caps daily for 7 days. For Prescriber: Your name. Total quantity: 14 and no refills. Allow substitutions Send the script to "MIE Test Pharmacy", for patient HART, WILLIAM S</t>
+  </si>
+  <si>
+    <t>verify text equals "HART, WILLIAM S." in "patient_name"
+verify text equals "amoxicillin 500 mg tablet" in "medicine"</t>
   </si>
 </sst>
 </file>
@@ -500,7 +497,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -533,16 +530,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -550,16 +547,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
@@ -567,16 +564,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
@@ -584,16 +581,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,11 +603,12 @@
     <hyperlink ref="D4" r:id="rId1" xr:uid="{04ED3031-8870-4330-81D1-8617DD329C46}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{FE524888-D6D2-4840-9416-D3F21926355F}"/>
     <hyperlink ref="D5" r:id="rId3" location="/home" xr:uid="{61F39757-003C-442B-9351-F4B4ED6C4A1F}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{A6C6713C-B6D3-49F1-936E-142294D2DF64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 D3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: updated master daily keywords
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8D8254-BD8C-40D7-BB83-5A6D28AEF79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2F0C53-2EA5-4619-B5A3-36A6BD626A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
   </si>
   <si>
     <t>verify text equals "HART, WILLIAM S." in "patient_name"
-verify text equals "amoxicillin 500 mg tablet" in "medicine"</t>
+verify text equals "amoxicillin 500 mg capsule" in "medicine"</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: updated final test
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEDF057-F92B-4D6B-AB7B-95BFAE242564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5AFCD1-296F-445C-9DAC-79F8D245B381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -558,50 +558,46 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{04ED3031-8870-4330-81D1-8617DD329C46}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{04ED3031-8870-4330-81D1-8617DD329C46}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{FE524888-D6D2-4840-9416-D3F21926355F}"/>
-    <hyperlink ref="D5" r:id="rId3" location="/home" xr:uid="{61F39757-003C-442B-9351-F4B4ED6C4A1F}"/>
+    <hyperlink ref="D4" r:id="rId3" location="/home" xr:uid="{61F39757-003C-442B-9351-F4B4ED6C4A1F}"/>
     <hyperlink ref="D3" r:id="rId4" xr:uid="{A6C6713C-B6D3-49F1-936E-142294D2DF64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: alignment of text to left
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5AFCD1-296F-445C-9DAC-79F8D245B381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D3DBA1-4CD8-4F85-90AE-A244AC962AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1245" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,6 @@
     <t>herbie_script</t>
   </si>
   <si>
-    <t>Select Hart, William S from the list
-go to the charter page</t>
-  </si>
-  <si>
     <t>https://workforcenow.adp.com/theme/index.html#/home</t>
   </si>
   <si>
@@ -84,7 +80,10 @@
 verify text equals "amoxicillin 500 mg capsule" in "medicine"</t>
   </si>
   <si>
-    <t>verify url equals "https://masterdaily.dev.webchart.app/webchart.cgi?f=chart&amp;s=pat&amp;pat_id=18"</t>
+    <t>Task: Select Hart, William S from the list go to the chart page</t>
+  </si>
+  <si>
+    <t>verify text equals "HART, WILLIAM S." in "patient_name"</t>
   </si>
 </sst>
 </file>
@@ -496,7 +495,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -529,30 +528,30 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>19</v>
@@ -563,16 +562,16 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
@@ -580,16 +579,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data from old laptop
</commit_message>
<xml_diff>
--- a/public/tasks.xlsx
+++ b/public/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svelte\Herbie_Usability_Tests\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hkonda/Desktop/herbie/Herbie_Usability_Tests/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA77DA6A-2E0E-4C30-A23C-1FE9F879A998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5FAB44-6099-664B-A383-F367F4DA3647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1245" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -63,13 +63,6 @@
 Task: Enter your name in the form and submit it in academy page.</t>
   </si>
   <si>
-    <t>http://18.219.226.248/academy.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify url equals "http://18.219.226.248/academy.html"
-</t>
-  </si>
-  <si>
     <t>https://masterdaily.dev.webchart.app/webchart.cgi</t>
   </si>
   <si>
@@ -84,6 +77,13 @@
   </si>
   <si>
     <t>verify text equals "HART, WILLIAM S." in "patient_name"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify url equals "http://localhost/academy.html"
+</t>
+  </si>
+  <si>
+    <t>http://localhost/academy.html</t>
   </si>
 </sst>
 </file>
@@ -495,18 +495,18 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="29.625" customWidth="1"/>
-    <col min="4" max="4" width="54.125" customWidth="1"/>
-    <col min="5" max="5" width="39.625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="54.1640625" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -534,13 +534,13 @@
         <v>12</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -565,16 +565,16 @@
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -582,13 +582,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>